<commit_message>
commiting all updated files
</commit_message>
<xml_diff>
--- a/Testdata/TC_Unit_Manipulation_26.xlsx
+++ b/Testdata/TC_Unit_Manipulation_26.xlsx
@@ -28,7 +28,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>zZgAAB+LCAAAAAAAAAPtXVuP48aV/itEPywSwGpedO/lKNCle0ZOq7vRUntm9qVRIkst7lCklpe+5C3weu0snNhYI8bu2gtvsl7YARLDGxtIMnbsB/+VqNt58l/YUyzeRVJiT3u6HdMYeMRzqSoWq875zjdFSfzR+UxlTrFhKrp2b4Pf5DYYrEm6rGgn9zZsa1Liaxs/aonb5xJWD5CBZtgCYwa8NHPr3FTubUwta77FsmdnZ5tn5U3dOGEFjuPZR4PdoTTFM1RSNNNCmoQ3fC95tddGS+zKswG2kIwsRD3vbfSH/c0uVqQeyAZIQyfY2OzYpqJh09zWLMVSsEk8DYws3O0NXqI31hI2a5u8yC7JA8uOragytYtYUrlrB93ikTLDLYETuBLXLHHVEc9vlctbVfCqNf/Bc/QNxV1kWkNsnCqSIxhaaDZ33LkmV+X5crkKvSUaQVvBBLTEfVU+xKeKieUuVlUz14yw7gNsSxbcdb7J5EQ25Os2dP0h3DfQfDpSLBXndd/RDSzBRF2r7z18tm+48zea74J2NFUM66KHLnK3dWRiY39OZiOfa0vs6ZrVVrFhHc3hoWIZnjkoWpZhY5FNUQZOPcWU4LOi2VhuTZBqhp0iSvGhbjwx50jCe7BhWdLGmabqSIaVZSmmpUhBp0sK8cDQ59AidN7RVXkHWnWNExR+y30Npph029H1J8HokpSiswac1QDPdIYsz3xJLg6n+tm+pl4M7bEpGcoYy72OZ52oE8nOc727tmnpMxhFIBKpLCQZDNgL+A82W1wj9rCkzJB6oMI8mq0yNBQRiG3b0ieK1dVVe6aZ3rBiUvEh3NQIn/s36V+L+/B8NTLvutbXPHs604mqqMOhfub3uaxw5iEkbpuS98SXFXHjHsi8J7iscR4KucsdRYVcEH4cIWl0YQynGFuJq4JqRBL2dkh2aXUuSJ8iG0hEWJywwEHaIjmi5PwZcdyW8wd69tXitia7djxX4oVSOWznKcU9e7Y/hk186txTiwddTCTCXagdFWlPQPpQsaZ7bW/0CRqR3nOq/bJOhO06V9GFI/bnJSwT+5qk2jKmUaCvTZxFScZGH2OqWlwS7cLGbolIuxhdzCHqmsqWBR/ubUAe3jItAzL9RkvSbc0yLki4EFnXdJWPaY81pwOkru0zMfA/2QAwLnZsTerq8vq9yXR2jjTFWn+Eum3QGLi+izN7JBzaZg+TwOJE+rX9pTz3ZBq5zGcanumaIq0/2zDJZPTyNW7E9HbV2h6Y7q+17VVI5jTXkb2+tpsB6BCyW65u2qapS4qzWN3tIYf82ZQt08MTZKuAzCzIqyd+tI2Lxbb5JG4TFolHhurFvBbBvSYAX0mebUqAGAi425T0GRGwgDcfDkU2bE9gj4S3tZNdpJ3YACz8uBKX+xGXJMWRgTST3I6PI2LBN9lI9OIUxTctGrz2bWch0OClg1ZkY3biCM/muoHUAUyMsuMuOxckAf4YIGvqXkE2U7HkTTIbuPpe0ZF5A19l5qQlehtkw7thMiZ0jMi9UIgd2AQykdzlALal2kWqMjZoVPWSd5IOHliACL34S24uJzr0ngGUWZBvf4wvCPYOLly5s2R5T0EXMAmkreFhrVGtCw1SvZBr0bljmCIZMx2kkgoM8pwzC26mSTIIq8QdL1o7DQ5g0UUEUT3AhBMFcsGSna8I7FsDAI9T9SJkSce7q0tg+PWnf7z897cWf/jor7/+LzpmKhdHaKxip+9Rh2/UmjWYoUAmktlgHQAr25LlyO4/cHCrfy26dZZz0d3ud+/vdpwA4As9d5oDWFLCXeh2cDmkA3Y6cp4B6z06atIaeQHFvY5oQzmlRUqqUxy1DuvTHOlkXH32wdVnv0v1dmcsgp2qJa68BnYitW0taudjp91I0A4K4UrIOGYjHtKI7c9THwrtplAVKhxX8YOv7C/LJKO4ym1phE7YmB8VdSme8ZdA+NpTOmv8/hQ2pK+nyz50QWdx8a//ffX0k4iVO72uJNYMDM9BHqQ71rtw2u5A2GT0CePahzQhK9p2qqnbtb9zwktmeV9FFlSSlDaX6Rjv8b6h2/OlmBBIEywTo8OyNubpzMzy0AJdgj0d7OW7ryU5uHfSC8Bk62jYY2aav8QcmRjRUFFI727A//jiL3989eqLXyxeeTni7nbiF+GwXmFXhC/95Quhyw30MYn4cOhM5RPuOBTYXSGpYA50RbPMFl8TnOrFvRTBlyfNOX+L/RkkG6dlZ7ZAHpOID5C5fW65O7S1J7JRAQx0jiDP6UGd5wtoNA5F7V99yNx/sPliG4q0bz7/z3AQv/rsva8/+pUbq+PxnKYh8sl332IiaYkJ6IlQG2RwDhSIb1TofPH+29A/GW3MIuxDd+0WQ5gl5USjfUZ8fHOaYbt8oyxwZd/EzTr6XJGWg0VMHJh5wSIQUB3NawfQB1+tu2raAwEOY2SGZu6+qo+RyngKp1CPmUS8sh0CWxowd/c77d3AhA5i35ChrucI20A+iH3Tg2Le0ghJQAsQSbJVwqcsmS2rRO9TKOqwLjExacuEjm5xScV/xELs2oZBYYfmctpDew6w0WOw0vUOqxdCinsU1YWxY3Dd70X1cB3SQgaKqonA0TuBxFXRoNI3CQdCgd8emZrgEnQRJhCmw6WtKcQ5VeAxsCRQbBuGbiRGi0DjmQ0Ac0IEYIMZ921Y0iXFp3LwrDyBF6EKnFrg1AKnFji1wKm3gFOnchpOJZoUnJrgmB+h8ukIlT+G5d9AZQGVhMZEKFUmXKOEpCpXquJ6dVyu8LjBTW4DvHqPK4ElTx/E2snkWk8+azUmFB03HRbXzajZAXBVYFpd3bAZj6YoOYqSI1xy8H7J4UFWkzLKMZ4ZIobcOtrrj44H7b3+wdFue9TfJ6CapOxQdqEmR7uj/sFuf/vwBw9sTTaw/PcMrQosBqkqMyNE9lxVAHH/kFD+oeQUHIOhw/CvXYALe/IEWwO/AQ/nvoRUG7ce9ESWfnJgYKu7vzcctfcAjLn/GBFrMqkHNJ+rThxP62R0eLSdrxs2fFcUL8bRekjqP4kgerUNxZpCA4q0P8eUGYeds2znu5KqKHBikrycwiled7qhRKcO+Lp1CEuBPBuJiWws/MevvagVlrOhioANQX82CeezEWDPPjOIZ1PBd7rGG2mQPBIr64TckmiXBrkTjVdD7jhOdiTro2g2kp3YZZAciNhU+MsuoVw2GZOmiJdc/OWfKExaVT6ASBR6HYQgHUvxA7sMANmboSLZMGjingm3rZ/h2ZCAXc6+UREbyZ1sPE2GBWwoAbIJ2S4mY6PpinWjEvtdY8Hcvu8yDcZeh/hib47fCiWWnjKZPAZg+ig4oeMJ6IiDVsgFzalLoIQNoZbQ2nCP8dzsYrkOtklqpiBe8xKv6xfBd5OTLUONV+YbEU62a9hQEO0rKtMnZy8sM4mXTTDK4Gbb/Jrk7JJhEjv7GCMjlZxd/OK9y9//6esv31m88T+p5GwNCp/KKm62Pyq42dD5S15Y5/xlY8kunZvlmyWuXuKaOblZTmjytTInZHKzgVE6NwtP+LDTbh8G0OdkGWcGRkuaCI1LVksqjdu3EFmw2TTu5T+/sXj/g8Vrv8licqMtpTO5EO50DTMH2DJ0VZlAasumc7PtszjdtqbZSH2BwRrJCcxGD0sbhBjGSJoyF7BV87O912wynQd+nJsHTvTI5IGXotIaNPDiT5+uSQOPdI2xpkk0sKdJoYEXP3958eaHz0gDC+k0sHAcyiIJXG/jLp1T6I82Dzsc1yS8XShPwOXl6z9bvPvx4vWni9f+5er/PltNIHpNbTFLqXCL6Vww7g7NZhH9LU9YzJf/fPn0zVVEorP/t5htDRsnFwzR6EYmkUhS3QoeMRR40qlEN/CkUYm12goecfHKh1dvvnz5y48vf/7R4ulbz49HFL6jRxe+A0XbjUDoWAApcHKBkwucXODkAicXOPmaODn5uISnScHJCY75cXI5HSeXjysVqYLK9UlJFhpyqSLUcalRx5VSYyJwUq1cw+Vx9RYg9HqnJRoZhyWystZ1nnvWUkwoeW46/uZJ39nRdlVoe64HJora5/tX+5SLMxS3eYbCrxqKMxTFGYriDEVxhqI4Q1GcoSjOUBRnKP5mltyNMMDrl8Z3lByu1pvlSjVCDm+fu+XQS+RrnPAWc3CwxfQNKFz3Dcz8HZrNnYUlQVtkxyRyx/nbuBOvxy1efUrryr+++gb8/+CAfHzrp1fvfXn13ieLf3v96vdfwOd0zrlar9dWcc6dw4JzpgiTbzaa6303FnlBpJ7nvblGiavl5ZwrDfLiwgrO2TfK4Jw7hy+2e+1hNufsG2VzzmS1pHLOHQP9RFFXvmP3h0+//t8vsxjnWDvplPNA0RQTLAhT28OnWNXnM1hvLzB9TbYdBdJk/xWRDC6aNvTVbwxFZ2RE3L96Sr7+CL0AYWEGcgkU2+dQmCq6wWDG2Q5ffaCbxet639rrek9OUo5puIqMUxqv/Pby7fefkYCupBPQleNQplpmmcv15l06qdE5dN7Pqvqvd1H2jJCXofSymqr02vHe8wre79piYvl1xQtfTgBY+4UvGg3yvPHVrPMrXvdyQ1A6T+mFoFSiUrirL3tVikMadxqix4JHgcMLHF7g8AKHFzi8wOF3FocnHwNxFSk4fNktPwavpmPw6jGqcGUk8I2SUOcmpYrA10qImwilBsI8pK+GhNCtwPO1ToHEB3HL35kRKaluOhLfIADIDssrY+BzPSVS1F3fq7qrWhwQudUDIl7FUhwQKQ6IFAdEigMixQGR4oBIcUCkOCDyN7PkboR9Xr9svpvEdK3aaHC1CC/9g173hyu//DjB6E4wy998/trip+9e/u7Xl+98evn2x998/rO1vhK52WisJJR3nj+h3F2XUA7/2N51aWU6b3lo5aawHpnB5XqlsEIaFbh8tHK9ztf4OsdnscqBTQapvHP4Yrvd7maTyr5RNqm8k0Uq7xh026x4o/CTXy7e+XMWqRxrJ51U3nN/Go3pa6alWLaFCb0csB8Op7wNy0ifQWE2tGxZwWY2vey1xPhtQ0BQkd8oLG8GWyA0mW1oj/xF2wdFQTF/exTz9tFhyi+IeJrMXxC5/O0Hz/4LIrV0rrl2HCSeZT5ZIF/te3eOe+xQulBYph332juMgU8ZfjXn6DWSxDkmNZP0UpoTCdZmG2lYyMU2NrgVL6S5sSidbfRiUSrbWL2rbGPtO3rK43vyZXbRiFFA6QJKF1C6gNIFlC6g9POA0snHNTxNCpROcMwPouvpILp+XJ5MJGkiNEpNCVdLlSovlcbNhlBqjFGNrzbLuMwlfvHdtw2w1zqwER/ELR/YiNZFNx2Z86T7zDi8Muo91xMZRWn0fSiN6sVBjFv9tRO3rCjOYRTnMIpzGMU5jOIcRnEOoziHUZzDKPjhED+8fjH8rXDH7oddqFsChNTDKuA55nymaua9jf6wv9nFikQCGW3A2OzYpqJB79uapVjgsxHkWn2gn17bF5ZFXte+ua/K7jzn8g2mJWgAIMu5hNX7BppPyRrKO5i2YQDCmGJsmXlddxXtST/f3bcQFjihwo3rk+q4UR+PhfpEapbrlaY8btYRrBraKKkFSBPkTawBLI58nfAkPoXdYZfrZ5qqI/kQaSc5W6MT7DjCYycz5exV4gSL0b8WdxTDtB4REOB+opLHvuQxBY6PWg2KDh/R68ctnpz9ph8BZIZ6YyPD9mKP5Zh0dXVXmSlWvpvhvAAVbQTWwXxOgWDeJ9rtDfbwuSWyoRYANIz/EfAJqQrytUa3FVRAvr/X1tAe526O9ZwPQE9W1vW8t2XAl9f3JhO9o6jPMAAHVV63ib5mKidTK+9zrdRQRSpXmqWxIE9KlTEul5q4XC41ypU6z3NVyABQKfuNQ+ZQ8FnOTki+UUwbqfn96D4JVfL/Dx7kGVPNmAAA</t>
+          <t>X5kAAB+LCAAAAAAAAAPtXVtv5MaV/iuEHhY24BbJvrfC6aAv0kx71ZKgbnlm9kWoJqsl7rDJXl502bfAcTwJnNhYI8bu2gvn4oUdIDG8sYEkY8d+8F9JS86T/8KeYvF+66ZGHmliGgNP81yqisWqc77zTbFb+OHZTGFOsG7ImnpnjV/n1hisipokq0d31ixzWuLraz9sC5tnIlb2kI5m2ARjBrxUY+PMkO+sHZvmfINlT09P108r65p+xJY5jmcfDLdH4jGeoZKsGiZSRbzmeUnLvdbaQk+aDbGJJGQi6nlnbTAarPewLPZBNkQqOsL6etcyZBUbxqZqyqaMDeKpY2TiXn/4Cr2xdnm9vs4LbEzuW3YtWZGoXciSyh076BaP5Rlul7kyV+JaJb465hobXHOj2livlxv/4jp6hsI2MswR1k9k0RaMTDSb2+5ci69yDa5ZbQhsohG05U9AW9hVpH18IhtY6mFFMXLNCOs8wI5owl3nm0xOYAO+TkNXH8JdHc2Px7Kp4LzuW5qORZioK/W9g093dWf+xvNt0I6PZd0876Pz3G0dGFjfnZPZyOfaFvqaanYUrJsHc3ioWIJnDoq2qVtYYFOUvlNfNkT4LKsWltpTpBhBp5BSuK/pj4w5EvEObFiWtHGqKhqSYGWZsmHKot9pTCHs6docWoTOu5oibUGrjnGCwmt5oMIUk267mvbIH12SUrDXgL0a4JnOkOmax+TC6Fg73VWV85E1MURdnmCp33WtE3UC2XmOd88yTG0Go/BFApUFJMMhew7/wWaLaoQ+FuUZUvYUmEejXYGGQgKhY5naVDZ7mmLNVMMdVkQq3IebGuMz7ya9a2EXnq9K5l1TB6prT2c6URV22NdOvT7jCnseAuKOIbpPPK6IGvdB5j7BuMZ+KOQut2QFckHwcQSk4YUxOsbYTFwVVCOQsLdFsku7e076FFhfIsDihAUO0jbJESX7z5jjNuw/0LOnFjZVybHjuRJfLlWCdq5S2LFmuxPYxCf2PbV50EVEAtyF0lWQ+gik92XzeKfjjj5BI9B7TrWP6wTYrnMFndtib16CMmGgioolYRoFBurUXpRkbPQxpqqFmGgbNnZbQOr5+HwOUdeQN0z4cGcN8vCGYeqQ6dfaomappn5OwoXAOqbLfAxrotodIGVln6mO/80CgHG+ZaliT5NW702is3OgyubqI9QsncbA1V3s2SPh0DL6mAQWO9Kv7C/muSdDz2U+U/FMU2Vx9dmGSSajl65wI4a7q1b2wHR/rWyvQDKnuY7s9ZXddECHkN1yddMxDE2U7cXqbA8p4M+mbJk+niJLAWRmQl498qJtVCx0jEdRm6BIONAVN+a1Ce41APiK0mxdBMRAwN26qM2IgAW8eX8ksEF7AntEvKkebSP1yAJg4cWVqNyLuCQpjnWkGuR2PBwRCb7JRoIbpyi+adPgtWvZC4EGLw20AhuxE8Z4Ntd0pAxhYuQtZ9k5IAnwxxCZx84VZDMFi+4ks76r5xUemTvwZWZ2WqK3QTa8EyYjQtuI3AuF2L6NLxPIXQ5hWyo9pMgTnUZVN3kn6eCB+YjQjb/k5nKiQ/cZQJkF+faf8TnB3v6FI7eXLO8q6AImgbQ92q83a41yk1Qv5Fqw7ximSMJMFymkAoM8Z8+Ck2mSDIIqYcuN1naDQ1h0IUFYDzDhSIZcELPzFL59ewjg8Vg5D1jS8W5rIhh+89mfL/7z7cWfPv77b/6HjpnKhTGaKNjue9zlm/VWHWbIlwlkNlgbwEqWaNqyu/ds3OpdC06dZV/0Nge9u9tdOwB4Qted5gCWlHDnmuVfjuiA7Y7sZ8C6j46atMduQHGuQ9pATmmTkuoEh62D+jRHOhmXn394+fkfUr2dGQthp1qJq6yAnUhtWw/bedhpOxS0vUKYqwaMIzbCPo3Y3jwNoNBulWvlKsdVveArecsyySiqcloaoyM24kdFPYpnvCUQvHaV9hq/ewwb0tPTZR+4oLO4+NmvLp98GrJypteRRJqB4dnIg3THuhd2210Im4w2ZRz7gCZgRdtONXW69nZOcMnE91VoQSVJaXOZjtEe7+qaNY/FBF+aYJkYHeLaiKc9M/Gh+boEezrYi/ceJzk4d9L3wWT7YNRnZqq3xGyZENJQUUDvbMD/+vJvf3798stfLF57NeTudOIV4bBeYVcEL73lC6HLCfQRiXB/ZE/lI+4wENgdIalg9jRZNY02Xy/b1YtzKYAvT5qz/xYGM0g2dsv2bIE8IhHuIWPzzHR2aHtHYMMCGOgcQZ7T/DrPE9BoHIjav/6IuXtv/eUOFGnffvHfwSB++fn733z8aydWR+M5TUPkk+e+wYTSEuPTE4E2yOBsKBDdqND54oN3oH8y2ohF0Ifu2g2GMEvykUr7DPl45jTD9vhmpcxVPBMn62hzWYwHi4jYN3ODhS+gOprX9qAPvtZw1LQHAhwmyAjM3F1FmyCFcRV2oR4xCXllO/i2NGBu73Y7274JHcSuLkFdzxG2gXwQBoYLxdylEZCAFiCSaCmET4mZxVWC+ykQdViHmJh2JEJHt7mk4j9kIfQsXaewQ3U47ZE1B9joMljpepvVCyDFHYrqgtjRvx70w3q4DmghA4XVRGDr7UDiqGhQGRiEA6HAb4dMjX8JuhATCNPh0NYU4pzI8BhYEig2dV3TE6OFr3HNhoA5IQKw/ox7NizpkuJTyX9WrsCNUAVOLXBqgVMLnFrg1BvAqcdSGk4lmhScmuCYH6Hy6QiVP2y2xFoFNSYlsVWelKoTqV6a1Fr1EqpNxBo/rSGuhW4CvLqPK4ElTx/EysnkSk8+azUmFB3XHRZXzajZAXBZYFpe3bAZj6YoOYqSI1hy8F7J4UJWgzLKEZ4ZIobUPtgZjA+HnZ3B3sF2ZzzYJaCapOxAdqEmB9vjwd72YHP/hXuWKulY+gFDqwKTQYrCzAiRPVdkQNwvEso/kJz8YzB0GN61A3BhTx5hc+g14OLcV5Bi4fa9vsDSTzYMbPd2d0bjzg6AMecfIyJNJvWA5nPFjuNpnYz3DzbzdcMG74rixShaD0i9J+FHr44um8fQgCzuzjFlxmHnxO08V1IV+U5MkpddOEXrTieUaNQBX7UOYSmQZ0MxkY2E/+i1G7WCcjZQEbAB6M8m4Xw2BOzZpwbxbCr4Tte4I/WTR2JlnZBbEu3SIHei8XLIHcXJtmR1FM2GshMbB8m+iE2Fv2wM5bLJmDRFHHPxln+iMGlVeQAiUeh2EIB0LMUPbBwAstdDRbJB0MQ9FW5bPcOzAQEbz75hERvKnWw0TQYFbCABsgnZLiJjw+mKdaIS+7yxYE7ft5kGY69CfLHXx28FEktfnk4fAjB94J/QcQV0xH4r5ILm1BgoYQOoJbA2nGM817tYroJtkpopiNe8xOvqRfDt5GQrUONV+GaIk+3pFhREu7LCDMjZC9NI4mUTjDK42Q6/IjkbM0xiZx9ipKeSs4tfvH/xx79889W7izd/m0rO1qHwqS7jZgfjgpsNnL/ky6ucv2zG7NK5Wb5V4holrpWTm+XKLb5e4cqZ3KxvlM7NwhPe73Y6+z70OYrjTN8opgnRuGS1pNK4AxORBZtN4178+M3FBx8uHv8ui8kNt5TO5EK401TM7GFT1xR5Cqktm87Nts/idDuqaiHlJQarJCcwa30srhFiGCPxmDmHrZqf7b1ik+k88MPcPHCiRyYPHItKK9DAi798tiINPNZUxjxOooFdTQoNvPj5q4u3PnpKGricTgOXDwNZJIHrbd6mcwqD8fp+l+NahLcL5Am4vHjjp4v3Plm88WTx+CeX//f5cgLRbWqDiaXCDaZ7zjg7NJtF9LY8YTFf/evFk7eWEYn2/t9gNlWsH50zRKPpmUQiSXVLeMRA4EmnEp3Ak0Yl1utLeMTFax9dvvXqxS8/ufj5x4snbz87HrH8nB5deA6KtmuB0JEAUuDkAicXOLnAyQVOLnDyFXFy8nEJV5OCkxMc8+PkSjpOrhzW8KTJcQ1UkjgklaqVhlhqcvV6CaNapdKYlCuVVusGIPRqpyWaGYclsrLWVZ571lJMKHmuO/7mSd/Z0XZZaHumByaK2uf7V/tUijMUN3mGwqsaijMUxRmK4gxFcYaiOENRnKEozlAUZyj+YZbctTDAq5fGt5QcrjValWotRA6/0O+9uHnmlESvkK9ywhvM3t4GM9CheN3VMfNPaDa3F5cI7ZFdk8gfX62dW/Ga3LdfPF786L2LP/zm4t3PLt755Nsvfrp4/QmtOP/++pvw/7098vHtH12+/9Xl+58u/uONyz9+CZ/T2ehao1FfxkZ39585G91blY0OflvbVTlpOqWrc9J8q9la7buzyAskjXzv1fF536vjqk3yYsMSTtozyuCku/svd/qdUTYn7Rllc9JkzaRy0l0d/busLH0H70+fffO/X2Ux0pF20inpoazKBlgQJrePT7CizWew6l5iBqpk2QqkSt4rJBlcNW3o69/pssZIiLh//YR8PRJ6CcLFDOQiKDbPoHCVNZ3BjL0pvv5QM4rX+b6z1/keHaUc43AUGac4Xvv9xTsfPCVBXU0nqKuHgUwWZ6ErjdY10tAPn/YkR3efvL/FV73Xvyi7RshNN8lcPH7rb08+sFNNNBEtpzjd9t33w/z3wjaYSD5mXgjG9ReXvDdmx4mV3xujQSPPi2OtBr/krTEnUqXTnW6kSuU7y7eV76wWZz1uNdKPxJgCzhdwvoDzBZwv4HwB559bOJ982sRRpMD5uFt+KF9Lh/K1wxbf4qpirVriEaqUqhOIGEislmGHY04Sy9NKo4FvAuWvdNgkOogb/mqOUGV23ZH4msFBdmheGgef6YGUooQrSrh4CVcrjqzc6JEVt/gpjqwUR1aKIyvFkZXiyEpxZKU4slIcWfmHWXLXQmSvXmHfTo67Xms2uXqM4l76dcwJRreUnF7pS5pbzeZSBnqrYKAjDHSrvBrvweV6ybFKGi1z+RjoRoOv8w2OzyKgfZsM/nlr/+VOp9PL5p89o2z+eSuLf97S6bZZ8o7jp79cvPvXLP450k46/7zj/FgbM1ANUzYtExMm2idDbPp5E5aRNoPCbGRakoyNbCbabYnx2oaAoCCvUVjeDDZBaDCb0B75i7YPioKN/u7Y6M2D/ZTfNHE1mb9pcvH7D5/+N03q6bR0/dBPPHHquUy+bPj2fFXIls0ecuU4O7nT2WJ0fMLwyylIt5EkCjKpmaTX5OxIsDLbSMNCLraxyS15Rc6JRelsoxuLUtnG2m39kuH6c3pg5Hvy9XrhiFFA6QJKF1C6gNIFlC6g9LOA0sknO1xNCpROcMwPohvpILpxyEl1rlzH0xJuVFul6rQilpq1SblUnooNNK1XqtUpdxMAe6WzHdFB3PDZjnBddN2ROU+6z4zDS6PeMz24UZRG34fSqFEcxLjR319xyoriHEZxDqM4h1GcwyjOYRTnMIpzGMU5jIIfDvDDqxfD3wl37HzYhrrFR0h9rACeY85mimrcWRuMBus9LIskkNEG9PWuZcgq9L6pmrIJPmt+rtWG2smVfWFZ5HUdGLuK5MxzLl9/WvwGALKciVi5q6P5MVlDeQfT0XVAGMcYm0Ze121ZfTTId/ft+qTZqNVRHeNJC9WbkxoWxWmjWUGIl7gm3BttlNQCpAny0tYQFke+TngSn4LusMu1U1XRkLSP1KOcrdEJth3hsZOZsvcqcYLF6F0LW7JumA8ICHA+UclDT/KQAscH7SZFhw/o9cM2T85+048AMgO9saFhu7HHtE16mrItz2Qz381wboAKNwLrYD6nQDDvE+31hzv4zBTYQAsAGib/CviEVAX5WqPbCiogz99ta2RNcjfHus57oCcr62remxLgy6t7k4nekpWnGICNKq/axEA15KNjM+9zlSbTZq1RnZS4KVcpVaUaKk2kKQnyHIcbtXKjJcGq9RqHzCHj05ydkHwjGxZS8vvRfRKo5P8f4mZ8cl+ZAAA=</t>
         </r>
       </text>
     </comment>
@@ -84,18 +84,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <i/>
       <sz val="11"/>
-      <color rgb="FFFF3A56"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF3A56"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,14 +487,14 @@
           <t>Crude Oil Imports</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Exports: Volume: PP: Iron Ore &amp; Concentrates</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Exports: Volume: PP: Iron Ore &amp; Concentrates</t>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>(DC)Exports: Volume: PP: Iron Ore &amp; Concentrates</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>(DC)Exports: Volume: PP: Iron Ore &amp; Concentrates</t>
         </is>
       </c>
       <c r="H1" s="3" t="inlineStr">
@@ -534,12 +534,12 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Brazil</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Brazil</t>
         </is>
@@ -565,8 +565,8 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
@@ -596,12 +596,12 @@
           <t>Annual, ending "Dec" of each year</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
@@ -643,12 +643,12 @@
           <t>Ton hd</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>kg th</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>kg hd</t>
         </is>
@@ -690,12 +690,12 @@
           <t>Unione Petrolifera</t>
         </is>
       </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Ministry of Development, Industry and Trade</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>Ministry of Development, Industry and Trade</t>
         </is>
@@ -737,14 +737,14 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>Active</t>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
@@ -780,12 +780,12 @@
           <t>202916302 (ITRBAAR)</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>204883202 (BRJADAS)</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="G8" s="5" t="inlineStr">
         <is>
           <t>204883202 (BRJADAS)</t>
         </is>
@@ -827,12 +827,12 @@
           <t>SR3400318</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>SR3579345</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
+      <c r="G9" s="3" t="inlineStr">
         <is>
           <t>SR3579345</t>
         </is>
@@ -866,8 +866,8 @@
           <t>IT.NGSUPIMOIL.VO.TH-A</t>
         </is>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
@@ -889,8 +889,8 @@
           <t>UNIT_MULTIPLIER(Hundred; Convert all multipliers)</t>
         </is>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="inlineStr">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>UNIT_MULTIPLIER(Hundred; Convert all multipliers)</t>
         </is>
@@ -920,10 +920,10 @@
       <c r="E12" s="6">
         <v>37226</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="7">
         <v>32509</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="7">
         <v>32509</v>
       </c>
       <c r="H12" s="7">
@@ -951,10 +951,10 @@
       <c r="E13" s="6">
         <v>43435</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="7">
         <v>44013</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <v>44013</v>
       </c>
       <c r="H13" s="7">
@@ -982,11 +982,11 @@
       <c r="E14" s="8">
         <v>43655</v>
       </c>
-      <c r="F14" s="8">
-        <v>44049</v>
-      </c>
-      <c r="G14" s="8">
-        <v>44049</v>
+      <c r="F14" s="9">
+        <v>44088</v>
+      </c>
+      <c r="G14" s="9">
+        <v>44088</v>
       </c>
       <c r="H14" s="9">
         <v>41659</v>
@@ -1005,8 +1005,16 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="F15" s="11" t="inlineStr">
+        <is>
+          <t>Foreign Trade Secretariat started to adopt only international product classifications maintained by the UN. Both the Factor Aggregate and Product Group classification do not have a clear methodology, do not have national (IBGE) and international (UN) comparability and do not have revisions, preserving distortions in relation to the Harmonized System and changes in the Brazilian agenda. The related series had been reclassified to Economic Activity classification.</t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t>Foreign Trade Secretariat started to adopt only international product classifications maintained by the UN. Both the Factor Aggregate and Product Group classification do not have a clear methodology, do not have national (IBGE) and international (UN) comparability and do not have revisions, preserving distortions in relation to the Harmonized System and changes in the Brazilian agenda. The related series had been reclassified to Economic Activity classification.</t>
+        </is>
+      </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
@@ -1020,8 +1028,8 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
@@ -1043,10 +1051,10 @@
       <c r="E17" s="2">
         <v>836839</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>19191759.73266667</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <v>191917597.3266667</v>
       </c>
       <c r="H17" s="3">
@@ -1074,10 +1082,10 @@
       <c r="E18" s="2">
         <v>1835158943.333333</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>31494578560105.18</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <v>3149457856010518</v>
       </c>
       <c r="H18" s="3">
@@ -1105,10 +1113,10 @@
       <c r="E19" s="2">
         <v>42838.75515620562</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>5612003.079124706</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <v>56120030.79124706</v>
       </c>
       <c r="H19" s="3">
@@ -1136,10 +1144,10 @@
       <c r="E20" s="2">
         <v>-0.4036898088324275</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>0.1404455778312001</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>0.1404455778312033</v>
       </c>
       <c r="H20" s="3">
@@ -1167,10 +1175,10 @@
       <c r="E21" s="2">
         <v>-0.7938708325659465</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <v>-0.1951645620704356</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="3">
         <v>-0.1951645620704365</v>
       </c>
       <c r="H21" s="3">
@@ -1198,10 +1206,10 @@
       <c r="E22" s="2">
         <v>0.05119115523560161</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="3">
         <v>0.2924173268787023</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <v>0.2924173268787024</v>
       </c>
       <c r="H22" s="3">
@@ -1229,10 +1237,10 @@
       <c r="E23" s="2">
         <v>762170</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>3981355.53</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>39813555.3</v>
       </c>
       <c r="H23" s="3">
@@ -1260,10 +1268,10 @@
       <c r="E24" s="2">
         <v>893160</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="3">
         <v>35113043.186</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="3">
         <v>351130431.86</v>
       </c>
       <c r="H24" s="3">
@@ -1291,10 +1299,10 @@
       <c r="E25" s="2">
         <v>835830</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>18889023.017</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <v>188890230.17</v>
       </c>
       <c r="H25" s="3">
@@ -1322,10 +1330,10 @@
       <c r="E26" s="2">
         <v>10</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>120</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <v>120</v>
       </c>
       <c r="H26" s="3">
@@ -1343,16 +1351,16 @@
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="13">
+      <c r="F27" s="14">
         <v>16422155.327</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="14">
         <v>164221553.27</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="15">
         <v>-2621</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="15">
         <v>-26210000</v>
       </c>
     </row>
@@ -1364,16 +1372,16 @@
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="13">
+      <c r="F28" s="14">
         <v>10154487.387</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="14">
         <v>101544873.87</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="15">
         <v>-576</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="15">
         <v>-5760000</v>
       </c>
     </row>
@@ -1385,16 +1393,16 @@
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="13">
+      <c r="F29" s="14">
         <v>14599685.58</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="14">
         <v>145996855.8</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="15">
         <v>-108</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="15">
         <v>-1080000</v>
       </c>
     </row>
@@ -1406,16 +1414,16 @@
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
-      <c r="F30" s="13">
+      <c r="F30" s="14">
         <v>11118108.599</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="14">
         <v>111181085.99</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="15">
         <v>-1155</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="15">
         <v>-11550000</v>
       </c>
     </row>
@@ -1427,16 +1435,16 @@
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="13">
+      <c r="F31" s="14">
         <v>14317170.779</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="14">
         <v>143171707.79</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="15">
         <v>-1504</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="15">
         <v>-15040000</v>
       </c>
     </row>
@@ -1448,16 +1456,16 @@
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
-      <c r="F32" s="13">
+      <c r="F32" s="14">
         <v>11919311.414</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="14">
         <v>119193114.14</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="15">
         <v>-51</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="15">
         <v>-510000</v>
       </c>
     </row>
@@ -1469,16 +1477,16 @@
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="13">
+      <c r="F33" s="14">
         <v>15363976.165</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="14">
         <v>153639761.65</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="15">
         <v>-194</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="15">
         <v>-1940000</v>
       </c>
     </row>
@@ -1490,16 +1498,16 @@
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
-      <c r="F34" s="13">
+      <c r="F34" s="14">
         <v>13089065.497</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="14">
         <v>130890654.97</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="15">
         <v>-735</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="15">
         <v>-7350000</v>
       </c>
     </row>
@@ -1511,16 +1519,16 @@
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="13">
+      <c r="F35" s="14">
         <v>11590742.662</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="14">
         <v>115907426.62</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="15">
         <v>-495</v>
       </c>
-      <c r="I35" s="14">
+      <c r="I35" s="15">
         <v>-4950000</v>
       </c>
     </row>
@@ -1532,16 +1540,16 @@
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="13">
+      <c r="F36" s="14">
         <v>14378905.827</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="14">
         <v>143789058.27</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="14">
         <v>1103</v>
       </c>
-      <c r="I36" s="15">
+      <c r="I36" s="14">
         <v>11030000</v>
       </c>
     </row>
@@ -1553,16 +1561,16 @@
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
-      <c r="F37" s="13">
+      <c r="F37" s="14">
         <v>11774221.862</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="14">
         <v>117742218.62</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <v>161</v>
       </c>
-      <c r="I37" s="15">
+      <c r="I37" s="14">
         <v>1610000</v>
       </c>
     </row>
@@ -1578,16 +1586,16 @@
       <c r="E38" s="13">
         <v>828290</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="14">
         <v>11010233.944</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="14">
         <v>110102339.44</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="15">
         <v>-957</v>
       </c>
-      <c r="I38" s="14">
+      <c r="I38" s="15">
         <v>-9570000</v>
       </c>
     </row>
@@ -1599,16 +1607,16 @@
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="13">
+      <c r="F39" s="14">
         <v>12401093.962</v>
       </c>
-      <c r="G39" s="13">
+      <c r="G39" s="14">
         <v>124010939.62</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="15">
         <v>-1299</v>
       </c>
-      <c r="I39" s="14">
+      <c r="I39" s="15">
         <v>-12990000</v>
       </c>
     </row>
@@ -1620,16 +1628,16 @@
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="13">
+      <c r="F40" s="14">
         <v>10774785.141</v>
       </c>
-      <c r="G40" s="13">
+      <c r="G40" s="14">
         <v>107747851.41</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="15">
         <v>-751</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="15">
         <v>-7510000</v>
       </c>
     </row>
@@ -1641,16 +1649,16 @@
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="13">
+      <c r="F41" s="14">
         <v>12367971.427</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="14">
         <v>123679714.27</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="15">
         <v>-523</v>
       </c>
-      <c r="I41" s="14">
+      <c r="I41" s="15">
         <v>-5230000</v>
       </c>
     </row>
@@ -1662,16 +1670,16 @@
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="13">
+      <c r="F42" s="14">
         <v>14417822.884</v>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="14">
         <v>144178228.84</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42" s="14">
         <v>486</v>
       </c>
-      <c r="I42" s="15">
+      <c r="I42" s="14">
         <v>4860000</v>
       </c>
     </row>
@@ -1683,16 +1691,16 @@
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="13">
+      <c r="F43" s="14">
         <v>10517929.013</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="14">
         <v>105179290.13</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="15">
         <v>-604</v>
       </c>
-      <c r="I43" s="14">
+      <c r="I43" s="15">
         <v>-6040000</v>
       </c>
     </row>
@@ -1704,16 +1712,16 @@
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="13">
+      <c r="F44" s="14">
         <v>3981355.53</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="14">
         <v>39813555.3</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H44" s="14">
         <v>210</v>
       </c>
-      <c r="I44" s="15">
+      <c r="I44" s="14">
         <v>2100000</v>
       </c>
     </row>
@@ -1725,16 +1733,16 @@
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="13">
+      <c r="F45" s="14">
         <v>22754489.478</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="14">
         <v>227544894.78</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="14">
         <v>109</v>
       </c>
-      <c r="I45" s="15">
+      <c r="I45" s="14">
         <v>1090000</v>
       </c>
     </row>
@@ -1746,16 +1754,16 @@
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
-      <c r="F46" s="13">
+      <c r="F46" s="14">
         <v>20146610.381</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="14">
         <v>201466103.81</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="15">
         <v>-846</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="15">
         <v>-8460000</v>
       </c>
     </row>
@@ -1767,16 +1775,16 @@
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="13">
+      <c r="F47" s="14">
         <v>18190594.054</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="14">
         <v>181905940.54</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="15">
         <v>-405</v>
       </c>
-      <c r="I47" s="14">
+      <c r="I47" s="15">
         <v>-4050000</v>
       </c>
     </row>
@@ -1788,16 +1796,16 @@
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
-      <c r="F48" s="13">
+      <c r="F48" s="14">
         <v>14511446.132</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="14">
         <v>145114461.32</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="14">
         <v>567</v>
       </c>
-      <c r="I48" s="15">
+      <c r="I48" s="14">
         <v>5670000</v>
       </c>
     </row>
@@ -1809,16 +1817,16 @@
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
-      <c r="F49" s="13">
+      <c r="F49" s="14">
         <v>13714024.277</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="14">
         <v>137140242.77</v>
       </c>
-      <c r="H49" s="14">
+      <c r="H49" s="15">
         <v>-775</v>
       </c>
-      <c r="I49" s="14">
+      <c r="I49" s="15">
         <v>-7750000</v>
       </c>
     </row>
@@ -1834,16 +1842,16 @@
       <c r="E50" s="13">
         <v>809540</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F50" s="14">
         <v>12749376.333</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="14">
         <v>127493763.33</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H50" s="14">
         <v>467</v>
       </c>
-      <c r="I50" s="15">
+      <c r="I50" s="14">
         <v>4670000</v>
       </c>
     </row>
@@ -1855,16 +1863,16 @@
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="13">
+      <c r="F51" s="14">
         <v>16034142.275</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="14">
         <v>160341422.75</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="15">
         <v>-1791</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="15">
         <v>-17910000</v>
       </c>
     </row>
@@ -1876,16 +1884,16 @@
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
-      <c r="F52" s="13">
+      <c r="F52" s="14">
         <v>14533708.012</v>
       </c>
-      <c r="G52" s="13">
+      <c r="G52" s="14">
         <v>145337080.12</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="15">
         <v>-930</v>
       </c>
-      <c r="I52" s="14">
+      <c r="I52" s="15">
         <v>-9300000</v>
       </c>
     </row>
@@ -1897,16 +1905,16 @@
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
-      <c r="F53" s="13">
+      <c r="F53" s="14">
         <v>14713814.993</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="14">
         <v>147138149.93</v>
       </c>
-      <c r="H53" s="14">
+      <c r="H53" s="15">
         <v>-595</v>
       </c>
-      <c r="I53" s="14">
+      <c r="I53" s="15">
         <v>-5950000</v>
       </c>
     </row>
@@ -1918,16 +1926,16 @@
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="13">
+      <c r="F54" s="14">
         <v>16030445.694</v>
       </c>
-      <c r="G54" s="13">
+      <c r="G54" s="14">
         <v>160304456.94</v>
       </c>
-      <c r="H54" s="14">
+      <c r="H54" s="15">
         <v>-563</v>
       </c>
-      <c r="I54" s="14">
+      <c r="I54" s="15">
         <v>-5630000</v>
       </c>
     </row>
@@ -1939,16 +1947,16 @@
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
-      <c r="F55" s="13">
+      <c r="F55" s="14">
         <v>15793777.123</v>
       </c>
-      <c r="G55" s="13">
+      <c r="G55" s="14">
         <v>157937771.23</v>
       </c>
-      <c r="H55" s="14">
+      <c r="H55" s="15">
         <v>-1246</v>
       </c>
-      <c r="I55" s="14">
+      <c r="I55" s="15">
         <v>-12460000</v>
       </c>
     </row>
@@ -1960,16 +1968,16 @@
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
-      <c r="F56" s="13">
+      <c r="F56" s="14">
         <v>12093966.441</v>
       </c>
-      <c r="G56" s="13">
+      <c r="G56" s="14">
         <v>120939664.41</v>
       </c>
-      <c r="H56" s="14">
+      <c r="H56" s="15">
         <v>-421</v>
       </c>
-      <c r="I56" s="14">
+      <c r="I56" s="15">
         <v>-4210000</v>
       </c>
     </row>
@@ -1981,16 +1989,16 @@
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="13"/>
-      <c r="F57" s="13">
+      <c r="F57" s="14">
         <v>12550164.8</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="14">
         <v>125501648</v>
       </c>
-      <c r="H57" s="15">
+      <c r="H57" s="14">
         <v>477</v>
       </c>
-      <c r="I57" s="15">
+      <c r="I57" s="14">
         <v>4770000</v>
       </c>
     </row>
@@ -2002,16 +2010,16 @@
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="13"/>
-      <c r="F58" s="13">
+      <c r="F58" s="14">
         <v>11277423.428</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="14">
         <v>112774234.28</v>
       </c>
-      <c r="H58" s="14">
+      <c r="H58" s="15">
         <v>-1276</v>
       </c>
-      <c r="I58" s="14">
+      <c r="I58" s="15">
         <v>-12760000</v>
       </c>
     </row>
@@ -2023,16 +2031,16 @@
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13"/>
-      <c r="F59" s="13">
+      <c r="F59" s="14">
         <v>18305870.505</v>
       </c>
-      <c r="G59" s="13">
+      <c r="G59" s="14">
         <v>183058705.05</v>
       </c>
-      <c r="H59" s="14">
+      <c r="H59" s="15">
         <v>-575</v>
       </c>
-      <c r="I59" s="14">
+      <c r="I59" s="15">
         <v>-5750000</v>
       </c>
     </row>
@@ -2044,16 +2052,16 @@
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13"/>
-      <c r="F60" s="13">
+      <c r="F60" s="14">
         <v>20798586.244</v>
       </c>
-      <c r="G60" s="13">
+      <c r="G60" s="14">
         <v>207985862.44</v>
       </c>
-      <c r="H60" s="14">
+      <c r="H60" s="15">
         <v>-55</v>
       </c>
-      <c r="I60" s="14">
+      <c r="I60" s="15">
         <v>-550000</v>
       </c>
     </row>
@@ -2065,16 +2073,16 @@
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
-      <c r="F61" s="13">
+      <c r="F61" s="14">
         <v>13544806.035</v>
       </c>
-      <c r="G61" s="13">
+      <c r="G61" s="14">
         <v>135448060.35</v>
       </c>
-      <c r="H61" s="14">
+      <c r="H61" s="15">
         <v>-522</v>
       </c>
-      <c r="I61" s="14">
+      <c r="I61" s="15">
         <v>-5220000</v>
       </c>
     </row>
@@ -2090,16 +2098,16 @@
       <c r="E62" s="13">
         <v>843370</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="14">
         <v>9169338.135</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="14">
         <v>91693381.34999999</v>
       </c>
-      <c r="H62" s="15">
+      <c r="H62" s="14">
         <v>614</v>
       </c>
-      <c r="I62" s="15">
+      <c r="I62" s="14">
         <v>6140000</v>
       </c>
     </row>
@@ -2111,16 +2119,16 @@
       <c r="C63" s="13"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
-      <c r="F63" s="13">
+      <c r="F63" s="14">
         <v>21351993.727</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="14">
         <v>213519937.27</v>
       </c>
-      <c r="H63" s="14">
+      <c r="H63" s="15">
         <v>-1706</v>
       </c>
-      <c r="I63" s="14">
+      <c r="I63" s="15">
         <v>-17060000</v>
       </c>
     </row>
@@ -2132,16 +2140,16 @@
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
-      <c r="F64" s="13">
+      <c r="F64" s="14">
         <v>14418464.527</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="14">
         <v>144184645.27</v>
       </c>
-      <c r="H64" s="14">
+      <c r="H64" s="15">
         <v>-832</v>
       </c>
-      <c r="I64" s="14">
+      <c r="I64" s="15">
         <v>-8320000</v>
       </c>
     </row>
@@ -2153,16 +2161,16 @@
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
-      <c r="F65" s="13">
+      <c r="F65" s="14">
         <v>21632676.051</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="14">
         <v>216326760.51</v>
       </c>
-      <c r="H65" s="14">
+      <c r="H65" s="15">
         <v>-272</v>
       </c>
-      <c r="I65" s="14">
+      <c r="I65" s="15">
         <v>-2720000</v>
       </c>
     </row>
@@ -2174,16 +2182,16 @@
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
-      <c r="F66" s="13">
+      <c r="F66" s="14">
         <v>9175340.596999999</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="14">
         <v>91753405.97</v>
       </c>
-      <c r="H66" s="14">
+      <c r="H66" s="15">
         <v>-755</v>
       </c>
-      <c r="I66" s="14">
+      <c r="I66" s="15">
         <v>-7550000</v>
       </c>
     </row>
@@ -2195,16 +2203,16 @@
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
-      <c r="F67" s="13">
+      <c r="F67" s="14">
         <v>11966408.28</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="14">
         <v>119664082.8</v>
       </c>
-      <c r="H67" s="14">
+      <c r="H67" s="15">
         <v>-1713</v>
       </c>
-      <c r="I67" s="14">
+      <c r="I67" s="15">
         <v>-17130000</v>
       </c>
     </row>
@@ -2216,16 +2224,16 @@
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
-      <c r="F68" s="13">
+      <c r="F68" s="14">
         <v>16393408.469</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="14">
         <v>163934084.69</v>
       </c>
-      <c r="H68" s="14">
+      <c r="H68" s="15">
         <v>-1237</v>
       </c>
-      <c r="I68" s="14">
+      <c r="I68" s="15">
         <v>-12370000</v>
       </c>
     </row>
@@ -2237,16 +2245,16 @@
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
-      <c r="F69" s="13">
+      <c r="F69" s="14">
         <v>21648891.535</v>
       </c>
-      <c r="G69" s="13">
+      <c r="G69" s="14">
         <v>216488915.35</v>
       </c>
-      <c r="H69" s="15">
+      <c r="H69" s="14">
         <v>13</v>
       </c>
-      <c r="I69" s="15">
+      <c r="I69" s="14">
         <v>130000</v>
       </c>
     </row>
@@ -2258,16 +2266,16 @@
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
-      <c r="F70" s="13">
+      <c r="F70" s="14">
         <v>22481829.256</v>
       </c>
-      <c r="G70" s="13">
+      <c r="G70" s="14">
         <v>224818292.56</v>
       </c>
-      <c r="H70" s="14">
+      <c r="H70" s="15">
         <v>-3520</v>
       </c>
-      <c r="I70" s="14">
+      <c r="I70" s="15">
         <v>-35200000</v>
       </c>
     </row>
@@ -2279,16 +2287,16 @@
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
-      <c r="F71" s="13">
+      <c r="F71" s="14">
         <v>18211531.104</v>
       </c>
-      <c r="G71" s="13">
+      <c r="G71" s="14">
         <v>182115311.04</v>
       </c>
-      <c r="H71" s="14">
+      <c r="H71" s="15">
         <v>-2051</v>
       </c>
-      <c r="I71" s="14">
+      <c r="I71" s="15">
         <v>-20510000</v>
       </c>
     </row>
@@ -2300,16 +2308,16 @@
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
-      <c r="F72" s="13">
+      <c r="F72" s="14">
         <v>17241884.161</v>
       </c>
-      <c r="G72" s="13">
+      <c r="G72" s="14">
         <v>172418841.61</v>
       </c>
-      <c r="H72" s="14">
+      <c r="H72" s="15">
         <v>-1719</v>
       </c>
-      <c r="I72" s="14">
+      <c r="I72" s="15">
         <v>-17190000</v>
       </c>
     </row>
@@ -2321,16 +2329,16 @@
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
-      <c r="F73" s="13">
+      <c r="F73" s="14">
         <v>19290371.612</v>
       </c>
-      <c r="G73" s="13">
+      <c r="G73" s="14">
         <v>192903716.12</v>
       </c>
-      <c r="H73" s="14">
+      <c r="H73" s="15">
         <v>-2843</v>
       </c>
-      <c r="I73" s="14">
+      <c r="I73" s="15">
         <v>-28430000</v>
       </c>
     </row>
@@ -2346,16 +2354,16 @@
       <c r="E74" s="13">
         <v>869710</v>
       </c>
-      <c r="F74" s="13">
+      <c r="F74" s="14">
         <v>17624761.9</v>
       </c>
-      <c r="G74" s="13">
+      <c r="G74" s="14">
         <v>176247619</v>
       </c>
-      <c r="H74" s="14">
+      <c r="H74" s="15">
         <v>-2471</v>
       </c>
-      <c r="I74" s="14">
+      <c r="I74" s="15">
         <v>-24710000</v>
       </c>
     </row>
@@ -2367,16 +2375,16 @@
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
-      <c r="F75" s="13">
+      <c r="F75" s="14">
         <v>15184509.886</v>
       </c>
-      <c r="G75" s="13">
+      <c r="G75" s="14">
         <v>151845098.86</v>
       </c>
-      <c r="H75" s="14">
+      <c r="H75" s="15">
         <v>-3034</v>
       </c>
-      <c r="I75" s="14">
+      <c r="I75" s="15">
         <v>-30340000</v>
       </c>
     </row>
@@ -2388,16 +2396,16 @@
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
-      <c r="F76" s="13">
+      <c r="F76" s="14">
         <v>17560691.672</v>
       </c>
-      <c r="G76" s="13">
+      <c r="G76" s="14">
         <v>175606916.72</v>
       </c>
-      <c r="H76" s="14">
+      <c r="H76" s="15">
         <v>-2300</v>
       </c>
-      <c r="I76" s="14">
+      <c r="I76" s="15">
         <v>-23000000</v>
       </c>
     </row>
@@ -2413,16 +2421,16 @@
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
-      <c r="F77" s="13">
+      <c r="F77" s="14">
         <v>17557605.651</v>
       </c>
-      <c r="G77" s="13">
+      <c r="G77" s="14">
         <v>175576056.51</v>
       </c>
-      <c r="H77" s="14">
+      <c r="H77" s="15">
         <v>-3374</v>
       </c>
-      <c r="I77" s="14">
+      <c r="I77" s="15">
         <v>-33740000</v>
       </c>
     </row>
@@ -2434,16 +2442,16 @@
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
-      <c r="F78" s="13">
+      <c r="F78" s="14">
         <v>19510789.765</v>
       </c>
-      <c r="G78" s="13">
+      <c r="G78" s="14">
         <v>195107897.65</v>
       </c>
-      <c r="H78" s="14">
+      <c r="H78" s="15">
         <v>-3151</v>
       </c>
-      <c r="I78" s="14">
+      <c r="I78" s="15">
         <v>-31510000</v>
       </c>
     </row>
@@ -2455,16 +2463,16 @@
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
-      <c r="F79" s="13">
+      <c r="F79" s="14">
         <v>17078551.013</v>
       </c>
-      <c r="G79" s="13">
+      <c r="G79" s="14">
         <v>170785510.13</v>
       </c>
-      <c r="H79" s="14">
+      <c r="H79" s="15">
         <v>-3342</v>
       </c>
-      <c r="I79" s="14">
+      <c r="I79" s="15">
         <v>-33420000</v>
       </c>
     </row>
@@ -2480,16 +2488,16 @@
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
-      <c r="F80" s="13">
+      <c r="F80" s="14">
         <v>18271416.025</v>
       </c>
-      <c r="G80" s="13">
+      <c r="G80" s="14">
         <v>182714160.25</v>
       </c>
-      <c r="H80" s="14">
+      <c r="H80" s="15">
         <v>-1667</v>
       </c>
-      <c r="I80" s="14">
+      <c r="I80" s="15">
         <v>-16670000</v>
       </c>
     </row>
@@ -2505,16 +2513,16 @@
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
-      <c r="F81" s="13">
+      <c r="F81" s="14">
         <v>18600783.758</v>
       </c>
-      <c r="G81" s="13">
+      <c r="G81" s="14">
         <v>186007837.58</v>
       </c>
-      <c r="H81" s="14">
+      <c r="H81" s="15">
         <v>-2237</v>
       </c>
-      <c r="I81" s="14">
+      <c r="I81" s="15">
         <v>-22370000</v>
       </c>
     </row>
@@ -2530,16 +2538,16 @@
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
-      <c r="F82" s="13">
+      <c r="F82" s="14">
         <v>20603806.861</v>
       </c>
-      <c r="G82" s="13">
+      <c r="G82" s="14">
         <v>206038068.61</v>
       </c>
-      <c r="H82" s="14">
+      <c r="H82" s="15">
         <v>-4281</v>
       </c>
-      <c r="I82" s="14">
+      <c r="I82" s="15">
         <v>-42810000</v>
       </c>
     </row>
@@ -2555,16 +2563,16 @@
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
-      <c r="F83" s="13">
+      <c r="F83" s="14">
         <v>18069058.618</v>
       </c>
-      <c r="G83" s="13">
+      <c r="G83" s="14">
         <v>180690586.18</v>
       </c>
-      <c r="H83" s="14">
+      <c r="H83" s="15">
         <v>-2394</v>
       </c>
-      <c r="I83" s="14">
+      <c r="I83" s="15">
         <v>-23940000</v>
       </c>
     </row>
@@ -2576,16 +2584,16 @@
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
-      <c r="F84" s="13">
+      <c r="F84" s="14">
         <v>18879562.08</v>
       </c>
-      <c r="G84" s="13">
+      <c r="G84" s="14">
         <v>188795620.8</v>
       </c>
-      <c r="H84" s="14">
+      <c r="H84" s="15">
         <v>-3020</v>
       </c>
-      <c r="I84" s="14">
+      <c r="I84" s="15">
         <v>-30200000</v>
       </c>
     </row>
@@ -2597,16 +2605,16 @@
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
-      <c r="F85" s="13">
+      <c r="F85" s="14">
         <v>20763765.22</v>
       </c>
-      <c r="G85" s="13">
+      <c r="G85" s="14">
         <v>207637652.2</v>
       </c>
-      <c r="H85" s="14">
+      <c r="H85" s="15">
         <v>-4417</v>
       </c>
-      <c r="I85" s="14">
+      <c r="I85" s="15">
         <v>-44170000</v>
       </c>
     </row>
@@ -2626,16 +2634,16 @@
       <c r="E86" s="13">
         <v>893160</v>
       </c>
-      <c r="F86" s="13">
+      <c r="F86" s="14">
         <v>22081603.935</v>
       </c>
-      <c r="G86" s="13">
+      <c r="G86" s="14">
         <v>220816039.35</v>
       </c>
-      <c r="H86" s="14">
+      <c r="H86" s="15">
         <v>-3481</v>
       </c>
-      <c r="I86" s="14">
+      <c r="I86" s="15">
         <v>-34810000</v>
       </c>
     </row>
@@ -2651,16 +2659,16 @@
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
-      <c r="F87" s="13">
+      <c r="F87" s="14">
         <v>17136921.055</v>
       </c>
-      <c r="G87" s="13">
+      <c r="G87" s="14">
         <v>171369210.55</v>
       </c>
-      <c r="H87" s="14">
+      <c r="H87" s="15">
         <v>-5007</v>
       </c>
-      <c r="I87" s="14">
+      <c r="I87" s="15">
         <v>-50070000</v>
       </c>
     </row>
@@ -2676,16 +2684,16 @@
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
-      <c r="F88" s="13">
+      <c r="F88" s="14">
         <v>17415842.842</v>
       </c>
-      <c r="G88" s="13">
+      <c r="G88" s="14">
         <v>174158428.42</v>
       </c>
-      <c r="H88" s="14">
+      <c r="H88" s="15">
         <v>-3141</v>
       </c>
-      <c r="I88" s="14">
+      <c r="I88" s="15">
         <v>-31410000</v>
       </c>
     </row>
@@ -2701,16 +2709,16 @@
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
-      <c r="F89" s="13">
+      <c r="F89" s="14">
         <v>23394978.648</v>
       </c>
-      <c r="G89" s="13">
+      <c r="G89" s="14">
         <v>233949786.48</v>
       </c>
-      <c r="H89" s="14">
+      <c r="H89" s="15">
         <v>-2739</v>
       </c>
-      <c r="I89" s="14">
+      <c r="I89" s="15">
         <v>-27390000</v>
       </c>
     </row>
@@ -2726,16 +2734,16 @@
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
-      <c r="F90" s="13">
+      <c r="F90" s="14">
         <v>15822450.66</v>
       </c>
-      <c r="G90" s="13">
+      <c r="G90" s="14">
         <v>158224506.6</v>
       </c>
-      <c r="H90" s="14">
+      <c r="H90" s="15">
         <v>-3655</v>
       </c>
-      <c r="I90" s="14">
+      <c r="I90" s="15">
         <v>-36550000</v>
       </c>
     </row>
@@ -2751,16 +2759,16 @@
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
-      <c r="F91" s="13">
+      <c r="F91" s="14">
         <v>13117250.978</v>
       </c>
-      <c r="G91" s="13">
+      <c r="G91" s="14">
         <v>131172509.78</v>
       </c>
-      <c r="H91" s="14">
+      <c r="H91" s="15">
         <v>-4317</v>
       </c>
-      <c r="I91" s="14">
+      <c r="I91" s="15">
         <v>-43170000</v>
       </c>
     </row>
@@ -2776,16 +2784,16 @@
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
-      <c r="F92" s="13">
+      <c r="F92" s="14">
         <v>20872630.854</v>
       </c>
-      <c r="G92" s="13">
+      <c r="G92" s="14">
         <v>208726308.54</v>
       </c>
-      <c r="H92" s="14">
+      <c r="H92" s="15">
         <v>-2250</v>
       </c>
-      <c r="I92" s="14">
+      <c r="I92" s="15">
         <v>-22500000</v>
       </c>
     </row>
@@ -2801,16 +2809,16 @@
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
-      <c r="F93" s="13">
+      <c r="F93" s="14">
         <v>29780925.685</v>
       </c>
-      <c r="G93" s="13">
+      <c r="G93" s="14">
         <v>297809256.85</v>
       </c>
-      <c r="H93" s="14">
+      <c r="H93" s="15">
         <v>-3408</v>
       </c>
-      <c r="I93" s="14">
+      <c r="I93" s="15">
         <v>-34080000</v>
       </c>
     </row>
@@ -2826,16 +2834,16 @@
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
-      <c r="F94" s="13">
+      <c r="F94" s="14">
         <v>22280138.559</v>
       </c>
-      <c r="G94" s="13">
+      <c r="G94" s="14">
         <v>222801385.59</v>
       </c>
-      <c r="H94" s="14">
+      <c r="H94" s="15">
         <v>-5544</v>
       </c>
-      <c r="I94" s="14">
+      <c r="I94" s="15">
         <v>-55440000</v>
       </c>
     </row>
@@ -2851,16 +2859,16 @@
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
-      <c r="F95" s="13">
+      <c r="F95" s="14">
         <v>20549065.387</v>
       </c>
-      <c r="G95" s="13">
+      <c r="G95" s="14">
         <v>205490653.87</v>
       </c>
-      <c r="H95" s="14">
+      <c r="H95" s="15">
         <v>-2196</v>
       </c>
-      <c r="I95" s="14">
+      <c r="I95" s="15">
         <v>-21960000</v>
       </c>
     </row>
@@ -2876,16 +2884,16 @@
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
-      <c r="F96" s="13">
+      <c r="F96" s="14">
         <v>22942420.007</v>
       </c>
-      <c r="G96" s="13">
+      <c r="G96" s="14">
         <v>229424200.07</v>
       </c>
-      <c r="H96" s="14">
+      <c r="H96" s="15">
         <v>-3289</v>
       </c>
-      <c r="I96" s="14">
+      <c r="I96" s="15">
         <v>-32890000</v>
       </c>
     </row>
@@ -2901,16 +2909,16 @@
       </c>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
-      <c r="F97" s="13">
+      <c r="F97" s="14">
         <v>20898332.317</v>
       </c>
-      <c r="G97" s="13">
+      <c r="G97" s="14">
         <v>208983323.17</v>
       </c>
-      <c r="H97" s="14">
+      <c r="H97" s="15">
         <v>-4019</v>
       </c>
-      <c r="I97" s="14">
+      <c r="I97" s="15">
         <v>-40190000</v>
       </c>
     </row>
@@ -2930,16 +2938,16 @@
       <c r="E98" s="13">
         <v>870060</v>
       </c>
-      <c r="F98" s="13">
+      <c r="F98" s="14">
         <v>18315785.54</v>
       </c>
-      <c r="G98" s="13">
+      <c r="G98" s="14">
         <v>183157855.4</v>
       </c>
-      <c r="H98" s="14">
+      <c r="H98" s="15">
         <v>-3689</v>
       </c>
-      <c r="I98" s="14">
+      <c r="I98" s="15">
         <v>-36890000</v>
       </c>
     </row>
@@ -2955,16 +2963,16 @@
       </c>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
-      <c r="F99" s="13">
+      <c r="F99" s="14">
         <v>22102204.307</v>
       </c>
-      <c r="G99" s="13">
+      <c r="G99" s="14">
         <v>221022043.07</v>
       </c>
-      <c r="H99" s="14">
+      <c r="H99" s="15">
         <v>-4958</v>
       </c>
-      <c r="I99" s="14">
+      <c r="I99" s="15">
         <v>-49580000</v>
       </c>
     </row>
@@ -2980,16 +2988,16 @@
       </c>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
-      <c r="F100" s="13">
+      <c r="F100" s="14">
         <v>19134819.769</v>
       </c>
-      <c r="G100" s="13">
+      <c r="G100" s="14">
         <v>191348197.69</v>
       </c>
-      <c r="H100" s="14">
+      <c r="H100" s="15">
         <v>-4205</v>
       </c>
-      <c r="I100" s="14">
+      <c r="I100" s="15">
         <v>-42050000</v>
       </c>
     </row>
@@ -3005,16 +3013,16 @@
       </c>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
-      <c r="F101" s="13">
+      <c r="F101" s="14">
         <v>21303470.283</v>
       </c>
-      <c r="G101" s="13">
+      <c r="G101" s="14">
         <v>213034702.83</v>
       </c>
-      <c r="H101" s="14">
+      <c r="H101" s="15">
         <v>-2253</v>
       </c>
-      <c r="I101" s="14">
+      <c r="I101" s="15">
         <v>-22530000</v>
       </c>
     </row>
@@ -3030,16 +3038,16 @@
       </c>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
-      <c r="F102" s="13">
+      <c r="F102" s="14">
         <v>20070776.946</v>
       </c>
-      <c r="G102" s="13">
+      <c r="G102" s="14">
         <v>200707769.46</v>
       </c>
-      <c r="H102" s="14">
+      <c r="H102" s="15">
         <v>-4310</v>
       </c>
-      <c r="I102" s="14">
+      <c r="I102" s="15">
         <v>-43100000</v>
       </c>
     </row>
@@ -3055,16 +3063,16 @@
       </c>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
-      <c r="F103" s="13">
+      <c r="F103" s="14">
         <v>22499797.667</v>
       </c>
-      <c r="G103" s="13">
+      <c r="G103" s="14">
         <v>224997976.67</v>
       </c>
-      <c r="H103" s="14">
+      <c r="H103" s="15">
         <v>-5226</v>
       </c>
-      <c r="I103" s="14">
+      <c r="I103" s="15">
         <v>-52260000</v>
       </c>
     </row>
@@ -3080,16 +3088,16 @@
       </c>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
-      <c r="F104" s="13">
+      <c r="F104" s="14">
         <v>18898483.954</v>
       </c>
-      <c r="G104" s="13">
+      <c r="G104" s="14">
         <v>188984839.54</v>
       </c>
-      <c r="H104" s="14">
+      <c r="H104" s="15">
         <v>-3917</v>
       </c>
-      <c r="I104" s="14">
+      <c r="I104" s="15">
         <v>-39170000</v>
       </c>
     </row>
@@ -3101,16 +3109,16 @@
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
-      <c r="F105" s="13">
+      <c r="F105" s="14">
         <v>27266930.595</v>
       </c>
-      <c r="G105" s="13">
+      <c r="G105" s="14">
         <v>272669305.95</v>
       </c>
-      <c r="H105" s="14">
+      <c r="H105" s="15">
         <v>-4817</v>
       </c>
-      <c r="I105" s="14">
+      <c r="I105" s="15">
         <v>-48170000</v>
       </c>
     </row>
@@ -3122,16 +3130,16 @@
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
-      <c r="F106" s="13">
+      <c r="F106" s="14">
         <v>24992028.138</v>
       </c>
-      <c r="G106" s="13">
+      <c r="G106" s="14">
         <v>249920281.38</v>
       </c>
-      <c r="H106" s="14">
+      <c r="H106" s="15">
         <v>-5252</v>
       </c>
-      <c r="I106" s="14">
+      <c r="I106" s="15">
         <v>-52520000</v>
       </c>
     </row>
@@ -3143,16 +3151,16 @@
       <c r="C107" s="13"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
-      <c r="F107" s="13">
+      <c r="F107" s="14">
         <v>22789512.526</v>
       </c>
-      <c r="G107" s="13">
+      <c r="G107" s="14">
         <v>227895125.26</v>
       </c>
-      <c r="H107" s="14">
+      <c r="H107" s="15">
         <v>-4295</v>
       </c>
-      <c r="I107" s="14">
+      <c r="I107" s="15">
         <v>-42950000</v>
       </c>
     </row>
@@ -3168,16 +3176,16 @@
       </c>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
-      <c r="F108" s="13">
+      <c r="F108" s="14">
         <v>25106766.211</v>
       </c>
-      <c r="G108" s="13">
+      <c r="G108" s="14">
         <v>251067662.11</v>
       </c>
-      <c r="H108" s="14">
+      <c r="H108" s="15">
         <v>-4534</v>
       </c>
-      <c r="I108" s="14">
+      <c r="I108" s="15">
         <v>-45340000</v>
       </c>
     </row>
@@ -3193,16 +3201,16 @@
       </c>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
-      <c r="F109" s="13">
+      <c r="F109" s="14">
         <v>22341102.397</v>
       </c>
-      <c r="G109" s="13">
+      <c r="G109" s="14">
         <v>223411023.97</v>
       </c>
-      <c r="H109" s="14">
+      <c r="H109" s="15">
         <v>-6653</v>
       </c>
-      <c r="I109" s="14">
+      <c r="I109" s="15">
         <v>-66530000</v>
       </c>
     </row>
@@ -3222,16 +3230,16 @@
       <c r="E110" s="13">
         <v>881580</v>
       </c>
-      <c r="F110" s="13">
+      <c r="F110" s="14">
         <v>22942124.617</v>
       </c>
-      <c r="G110" s="13">
+      <c r="G110" s="14">
         <v>229421246.17</v>
       </c>
-      <c r="H110" s="14">
+      <c r="H110" s="15">
         <v>-5259</v>
       </c>
-      <c r="I110" s="14">
+      <c r="I110" s="15">
         <v>-52590000</v>
       </c>
     </row>
@@ -3243,16 +3251,16 @@
       <c r="C111" s="13"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
-      <c r="F111" s="13">
+      <c r="F111" s="14">
         <v>24520920.568</v>
       </c>
-      <c r="G111" s="13">
+      <c r="G111" s="14">
         <v>245209205.68</v>
       </c>
-      <c r="H111" s="14">
+      <c r="H111" s="15">
         <v>-6447</v>
       </c>
-      <c r="I111" s="14">
+      <c r="I111" s="15">
         <v>-64470000</v>
       </c>
     </row>
@@ -3264,16 +3272,16 @@
       <c r="C112" s="13"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
-      <c r="F112" s="13">
+      <c r="F112" s="14">
         <v>23155257.304</v>
       </c>
-      <c r="G112" s="13">
+      <c r="G112" s="14">
         <v>231552573.04</v>
       </c>
-      <c r="H112" s="14">
+      <c r="H112" s="15">
         <v>-4037</v>
       </c>
-      <c r="I112" s="14">
+      <c r="I112" s="15">
         <v>-40370000</v>
       </c>
     </row>
@@ -3285,16 +3293,16 @@
       <c r="C113" s="13"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
-      <c r="F113" s="13">
+      <c r="F113" s="14">
         <v>14496817.17</v>
       </c>
-      <c r="G113" s="13">
+      <c r="G113" s="14">
         <v>144968171.7</v>
       </c>
-      <c r="H113" s="14">
+      <c r="H113" s="15">
         <v>-4754</v>
       </c>
-      <c r="I113" s="14">
+      <c r="I113" s="15">
         <v>-47540000</v>
       </c>
     </row>
@@ -3306,16 +3314,16 @@
       <c r="C114" s="13"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
-      <c r="F114" s="13">
+      <c r="F114" s="14">
         <v>17734886.761</v>
       </c>
-      <c r="G114" s="13">
+      <c r="G114" s="14">
         <v>177348867.61</v>
       </c>
-      <c r="H114" s="14">
+      <c r="H114" s="15">
         <v>-4869</v>
       </c>
-      <c r="I114" s="14">
+      <c r="I114" s="15">
         <v>-48690000</v>
       </c>
     </row>
@@ -3327,16 +3335,16 @@
       <c r="C115" s="13"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
-      <c r="F115" s="13">
+      <c r="F115" s="14">
         <v>35113043.186</v>
       </c>
-      <c r="G115" s="13">
+      <c r="G115" s="14">
         <v>351130431.86</v>
       </c>
-      <c r="H115" s="14">
+      <c r="H115" s="15">
         <v>-6337</v>
       </c>
-      <c r="I115" s="14">
+      <c r="I115" s="15">
         <v>-63370000</v>
       </c>
     </row>
@@ -3348,16 +3356,16 @@
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
-      <c r="F116" s="13">
+      <c r="F116" s="14">
         <v>25591778.512</v>
       </c>
-      <c r="G116" s="13">
+      <c r="G116" s="14">
         <v>255917785.12</v>
       </c>
-      <c r="H116" s="14">
+      <c r="H116" s="15">
         <v>-6381</v>
       </c>
-      <c r="I116" s="14">
+      <c r="I116" s="15">
         <v>-63810000</v>
       </c>
     </row>
@@ -3369,16 +3377,16 @@
       <c r="C117" s="13"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
-      <c r="F117" s="13">
+      <c r="F117" s="14">
         <v>27131551.809</v>
       </c>
-      <c r="G117" s="13">
+      <c r="G117" s="14">
         <v>271315518.09</v>
       </c>
-      <c r="H117" s="14">
+      <c r="H117" s="15">
         <v>-5364</v>
       </c>
-      <c r="I117" s="14">
+      <c r="I117" s="15">
         <v>-53640000</v>
       </c>
     </row>
@@ -3390,16 +3398,16 @@
       <c r="C118" s="13"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
-      <c r="F118" s="13">
+      <c r="F118" s="14">
         <v>26304268.183</v>
       </c>
-      <c r="G118" s="13">
+      <c r="G118" s="14">
         <v>263042681.83</v>
       </c>
-      <c r="H118" s="14">
+      <c r="H118" s="15">
         <v>-6916</v>
       </c>
-      <c r="I118" s="14">
+      <c r="I118" s="15">
         <v>-69160000</v>
       </c>
     </row>
@@ -3411,16 +3419,16 @@
       <c r="C119" s="13"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
-      <c r="F119" s="13">
+      <c r="F119" s="14">
         <v>29232786.719</v>
       </c>
-      <c r="G119" s="13">
+      <c r="G119" s="14">
         <v>292327867.19</v>
       </c>
-      <c r="H119" s="14">
+      <c r="H119" s="15">
         <v>-6104</v>
       </c>
-      <c r="I119" s="14">
+      <c r="I119" s="15">
         <v>-61040000</v>
       </c>
     </row>
@@ -3432,16 +3440,16 @@
       <c r="C120" s="13"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
-      <c r="F120" s="13">
+      <c r="F120" s="14">
         <v>26737568.449</v>
       </c>
-      <c r="G120" s="13">
+      <c r="G120" s="14">
         <v>267375684.49</v>
       </c>
-      <c r="H120" s="14">
+      <c r="H120" s="15">
         <v>-7140</v>
       </c>
-      <c r="I120" s="14">
+      <c r="I120" s="15">
         <v>-71400000</v>
       </c>
     </row>
@@ -3453,16 +3461,16 @@
       <c r="C121" s="13"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
-      <c r="F121" s="13">
+      <c r="F121" s="14">
         <v>17914269.559</v>
       </c>
-      <c r="G121" s="13">
+      <c r="G121" s="14">
         <v>179142695.59</v>
       </c>
-      <c r="H121" s="14">
+      <c r="H121" s="15">
         <v>-7067</v>
       </c>
-      <c r="I121" s="14">
+      <c r="I121" s="15">
         <v>-70670000</v>
       </c>
     </row>
@@ -3478,16 +3486,16 @@
       <c r="E122" s="13">
         <v>824320</v>
       </c>
-      <c r="F122" s="13">
+      <c r="F122" s="14">
         <v>13750599.7</v>
       </c>
-      <c r="G122" s="13">
+      <c r="G122" s="14">
         <v>137505997</v>
       </c>
-      <c r="H122" s="14">
+      <c r="H122" s="15">
         <v>-3233</v>
       </c>
-      <c r="I122" s="14">
+      <c r="I122" s="15">
         <v>-32330000</v>
       </c>
     </row>
@@ -3503,10 +3511,10 @@
       </c>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
-      <c r="F123" s="13">
+      <c r="F123" s="14">
         <v>17514932.668</v>
       </c>
-      <c r="G123" s="13">
+      <c r="G123" s="14">
         <v>175149326.68</v>
       </c>
       <c r="H123" s="13"/>
@@ -3524,10 +3532,10 @@
       </c>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
-      <c r="F124" s="13">
+      <c r="F124" s="14">
         <v>17479044.439</v>
       </c>
-      <c r="G124" s="13">
+      <c r="G124" s="14">
         <v>174790444.39</v>
       </c>
       <c r="H124" s="13"/>
@@ -3545,10 +3553,10 @@
       </c>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
-      <c r="F125" s="13">
+      <c r="F125" s="14">
         <v>22145797.118</v>
       </c>
-      <c r="G125" s="13">
+      <c r="G125" s="14">
         <v>221457971.18</v>
       </c>
       <c r="H125" s="13"/>
@@ -3566,10 +3574,10 @@
       </c>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
-      <c r="F126" s="13">
+      <c r="F126" s="14">
         <v>23474179.46</v>
       </c>
-      <c r="G126" s="13">
+      <c r="G126" s="14">
         <v>234741794.6</v>
       </c>
       <c r="H126" s="13"/>
@@ -3587,10 +3595,10 @@
       </c>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
-      <c r="F127" s="13">
+      <c r="F127" s="14">
         <v>15332000.414</v>
       </c>
-      <c r="G127" s="13">
+      <c r="G127" s="14">
         <v>153320004.14</v>
       </c>
       <c r="H127" s="13"/>
@@ -3608,10 +3616,10 @@
       </c>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
-      <c r="F128" s="13">
+      <c r="F128" s="14">
         <v>21381658.161</v>
       </c>
-      <c r="G128" s="13">
+      <c r="G128" s="14">
         <v>213816581.61</v>
       </c>
       <c r="H128" s="13"/>
@@ -3629,10 +3637,10 @@
       </c>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
-      <c r="F129" s="13">
+      <c r="F129" s="14">
         <v>25439411.944</v>
       </c>
-      <c r="G129" s="13">
+      <c r="G129" s="14">
         <v>254394119.44</v>
       </c>
       <c r="H129" s="13"/>
@@ -3650,10 +3658,10 @@
       </c>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
-      <c r="F130" s="13">
+      <c r="F130" s="14">
         <v>23297776.406</v>
       </c>
-      <c r="G130" s="13">
+      <c r="G130" s="14">
         <v>232977764.06</v>
       </c>
       <c r="H130" s="13"/>
@@ -3671,10 +3679,10 @@
       </c>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
-      <c r="F131" s="13">
+      <c r="F131" s="14">
         <v>28244132.638</v>
       </c>
-      <c r="G131" s="13">
+      <c r="G131" s="14">
         <v>282441326.38</v>
       </c>
       <c r="H131" s="13"/>
@@ -3688,10 +3696,10 @@
       <c r="C132" s="13"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
-      <c r="F132" s="13">
+      <c r="F132" s="14">
         <v>25624799.801</v>
       </c>
-      <c r="G132" s="13">
+      <c r="G132" s="14">
         <v>256247998.01</v>
       </c>
       <c r="H132" s="13"/>
@@ -3705,10 +3713,10 @@
       <c r="C133" s="13"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
-      <c r="F133" s="13">
+      <c r="F133" s="14">
         <v>21831171.984</v>
       </c>
-      <c r="G133" s="13">
+      <c r="G133" s="14">
         <v>218311719.84</v>
       </c>
       <c r="H133" s="13"/>
@@ -3726,10 +3734,10 @@
       <c r="E134" s="13">
         <v>762170</v>
       </c>
-      <c r="F134" s="13">
+      <c r="F134" s="14">
         <v>24188583.433</v>
       </c>
-      <c r="G134" s="13">
+      <c r="G134" s="14">
         <v>241885834.33</v>
       </c>
       <c r="H134" s="13"/>
@@ -3747,10 +3755,10 @@
       </c>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
-      <c r="F135" s="13">
+      <c r="F135" s="14">
         <v>21081548.368</v>
       </c>
-      <c r="G135" s="13">
+      <c r="G135" s="14">
         <v>210815483.68</v>
       </c>
       <c r="H135" s="13"/>
@@ -3768,10 +3776,10 @@
       </c>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
-      <c r="F136" s="13">
+      <c r="F136" s="14">
         <v>23422343.523</v>
       </c>
-      <c r="G136" s="13">
+      <c r="G136" s="14">
         <v>234223435.23</v>
       </c>
       <c r="H136" s="13"/>
@@ -3789,10 +3797,10 @@
       </c>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
-      <c r="F137" s="13">
+      <c r="F137" s="14">
         <v>27350943.882</v>
       </c>
-      <c r="G137" s="13">
+      <c r="G137" s="14">
         <v>273509438.82</v>
       </c>
       <c r="H137" s="13"/>
@@ -3810,10 +3818,10 @@
       </c>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
-      <c r="F138" s="13">
+      <c r="F138" s="14">
         <v>21363232.507</v>
       </c>
-      <c r="G138" s="13">
+      <c r="G138" s="14">
         <v>213632325.07</v>
       </c>
       <c r="H138" s="13"/>
@@ -3831,10 +3839,10 @@
       </c>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
-      <c r="F139" s="13">
+      <c r="F139" s="14">
         <v>23436747.168</v>
       </c>
-      <c r="G139" s="13">
+      <c r="G139" s="14">
         <v>234367471.68</v>
       </c>
       <c r="H139" s="13"/>
@@ -3852,10 +3860,10 @@
       </c>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
-      <c r="F140" s="13">
+      <c r="F140" s="14">
         <v>24450448.848</v>
       </c>
-      <c r="G140" s="13">
+      <c r="G140" s="14">
         <v>244504488.48</v>
       </c>
       <c r="H140" s="13"/>
@@ -3873,10 +3881,10 @@
       </c>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
-      <c r="F141" s="13">
+      <c r="F141" s="14">
         <v>25577795.131</v>
       </c>
-      <c r="G141" s="13">
+      <c r="G141" s="14">
         <v>255777951.31</v>
       </c>
       <c r="H141" s="13"/>
@@ -3894,10 +3902,10 @@
       </c>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
-      <c r="F142" s="13">
+      <c r="F142" s="14">
         <v>29786680.568</v>
       </c>
-      <c r="G142" s="13">
+      <c r="G142" s="14">
         <v>297866805.68</v>
       </c>
       <c r="H142" s="13"/>
@@ -3915,10 +3923,10 @@
       </c>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
-      <c r="F143" s="13">
+      <c r="F143" s="14">
         <v>27334052.404</v>
       </c>
-      <c r="G143" s="13">
+      <c r="G143" s="14">
         <v>273340524.04</v>
       </c>
       <c r="H143" s="13"/>
@@ -3936,10 +3944,10 @@
       </c>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
-      <c r="F144" s="13">
+      <c r="F144" s="14">
         <v>30184836.236</v>
       </c>
-      <c r="G144" s="13">
+      <c r="G144" s="14">
         <v>301848362.36</v>
       </c>
       <c r="H144" s="13"/>
@@ -3957,10 +3965,10 @@
       </c>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
-      <c r="F145" s="13">
+      <c r="F145" s="14">
         <v>24719201.999</v>
       </c>
-      <c r="G145" s="13">
+      <c r="G145" s="14">
         <v>247192019.99</v>
       </c>
       <c r="H145" s="13"/>
@@ -3982,10 +3990,10 @@
       <c r="E146" s="13">
         <v>786190</v>
       </c>
-      <c r="F146" s="13">
+      <c r="F146" s="14">
         <v>31980027.915</v>
       </c>
-      <c r="G146" s="13">
+      <c r="G146" s="14">
         <v>319800279.15</v>
       </c>
       <c r="H146" s="13"/>
@@ -4054,8 +4062,8 @@
           <InitCol>6</InitCol>
           <EndRow>146</EndRow>
           <EndCol>6</EndCol>
-          <Name>Exports: Volume: PP: Iron Ore &amp; Concentrates</Name>
-          <DisplayName>Exports: Volume: PP: Iron Ore &amp; Concentrates</DisplayName>
+          <Name>(DC)Exports: Volume: PP: Iron Ore &amp; Concentrates</Name>
+          <DisplayName>(DC)Exports: Volume: PP: Iron Ore &amp; Concentrates</DisplayName>
           <SeriesId>204883202</SeriesId>
           <Code>SR3579345</Code>
           <Order>4</Order>
@@ -4065,8 +4073,8 @@
           <InitCol>7</InitCol>
           <EndRow>146</EndRow>
           <EndCol>7</EndCol>
-          <Name>Exports: Volume: PP: Iron Ore &amp; Concentrates</Name>
-          <DisplayName>Exports: Volume: PP: Iron Ore &amp; Concentrates</DisplayName>
+          <Name>(DC)Exports: Volume: PP: Iron Ore &amp; Concentrates</Name>
+          <DisplayName>(DC)Exports: Volume: PP: Iron Ore &amp; Concentrates</DisplayName>
           <SeriesId>204883202</SeriesId>
           <Code>SR3579345</Code>
           <Order>5</Order>
@@ -4100,7 +4108,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{510192DB-6F2F-424A-BCAA-89AAD7B22808}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B12949-61C4-41E7-AB20-F2BFFDD41641}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
   </ds:schemaRefs>

</xml_diff>